<commit_message>
Add a bunch of additional notes.
</commit_message>
<xml_diff>
--- a/JWM_schedule.xlsx
+++ b/JWM_schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28300" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="25">
   <si>
     <t>Day</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>Eleocharis intraspecific variation</t>
+  </si>
+  <si>
+    <t>Roads &amp; seed dispersal</t>
+  </si>
+  <si>
+    <t>Chestnut morpotypes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Lakes thistle </t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>Concord B</t>
+  </si>
+  <si>
+    <t>Jessi</t>
+  </si>
+  <si>
+    <t>posters</t>
   </si>
 </sst>
 </file>
@@ -137,7 +158,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -147,8 +168,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -164,16 +193,27 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -597,6 +637,12 @@
         <f t="shared" ref="B6:B34" si="0">0.25+B5</f>
         <v>9.25</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
@@ -606,6 +652,12 @@
         <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
@@ -615,6 +667,11 @@
         <f t="shared" si="0"/>
         <v>9.75</v>
       </c>
+      <c r="C8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
@@ -624,6 +681,9 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
@@ -633,6 +693,9 @@
         <f t="shared" si="0"/>
         <v>10.25</v>
       </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
@@ -642,6 +705,9 @@
         <f t="shared" si="0"/>
         <v>10.5</v>
       </c>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
@@ -660,6 +726,12 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="4" t="s">
@@ -714,6 +786,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
+      <c r="C17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
@@ -723,6 +800,9 @@
         <f t="shared" si="0"/>
         <v>12.25</v>
       </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
@@ -732,6 +812,9 @@
         <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
@@ -741,6 +824,9 @@
         <f t="shared" si="0"/>
         <v>12.75</v>
       </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
@@ -750,6 +836,9 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
@@ -759,6 +848,9 @@
         <f t="shared" si="0"/>
         <v>13.25</v>
       </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="4" t="s">
@@ -804,6 +896,9 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
@@ -813,6 +908,9 @@
         <f t="shared" si="0"/>
         <v>14.25</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
@@ -822,6 +920,9 @@
         <f t="shared" si="0"/>
         <v>14.5</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="1" t="s">
@@ -831,6 +932,11 @@
         <f t="shared" si="0"/>
         <v>14.75</v>
       </c>
+      <c r="C28" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="1" t="s">
@@ -840,6 +946,9 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="1" t="s">
@@ -849,6 +958,9 @@
         <f t="shared" si="0"/>
         <v>15.25</v>
       </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="1" t="s">
@@ -858,6 +970,9 @@
         <f t="shared" si="0"/>
         <v>15.5</v>
       </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="1" t="s">
@@ -867,8 +982,11 @@
         <f t="shared" si="0"/>
         <v>15.75</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -876,8 +994,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -885,8 +1006,14 @@
         <f t="shared" si="0"/>
         <v>16.25</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -894,8 +1021,11 @@
         <f>0.25+B34</f>
         <v>16.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -905,6 +1035,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C17:E22"/>
+    <mergeCell ref="C8:E11"/>
+    <mergeCell ref="C28:E31"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>